<commit_message>
Committing the new update on pom.xml file
</commit_message>
<xml_diff>
--- a/TestData/AllTeacherTestDatas-DESKTOP-8AF4MIK.xlsx
+++ b/TestData/AllTeacherTestDatas-DESKTOP-8AF4MIK.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/1886f220f6a057ee/Desktop/Automation/AllTeachersPortalAutomationParallel4withseparate/TestData/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Hp\git\AllTeacherSeleniumArchitectGitHubActions\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="4" documentId="13_ncr:1_{87B5AFA6-BBA0-4AD5-B0AC-C9D82229D257}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{26A65F1E-79EE-4551-AA34-93F263334F3C}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E10AC73E-1D63-45E5-9552-AEAB58339ECF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1860" yWindow="1860" windowWidth="14400" windowHeight="7360" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="1" r:id="rId1"/>
@@ -583,7 +583,7 @@
     <t>அஓங்க்உ</t>
   </si>
   <si>
-    <t>https://allteacher.navadhiti.com/dashboar</t>
+    <t>https://allteacher.navadhiti.com/dashboard</t>
   </si>
 </sst>
 </file>
@@ -2513,7 +2513,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1D0B2F34-C77A-44EB-829F-BA8A4315E87C}">
   <dimension ref="A1:H3"/>
   <sheetViews>
-    <sheetView topLeftCell="F1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
       <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
@@ -2708,7 +2708,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0F3CC47E-5BAB-4B17-B0AA-D74228E5FC70}">
   <dimension ref="A1:L10"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+    <sheetView topLeftCell="F1" workbookViewId="0">
       <selection activeCell="L10" sqref="L10"/>
     </sheetView>
   </sheetViews>

</xml_diff>